<commit_message>
ok, working, happy with it
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="2"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="109">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>First-line treatment</t>
-  </si>
-  <si>
-    <t>Second-line treatment</t>
   </si>
   <si>
     <t>Death rate (% mortality per year)</t>
@@ -1978,7 +1975,7 @@
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2329,9 +2326,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2789,18 +2788,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="15">
-        <v>0.16</v>
-      </c>
-      <c r="D46" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="E46" s="15">
-        <v>0.26</v>
-      </c>
+      <c r="B46" s="3"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
@@ -2809,29 +2797,40 @@
       <c r="B48" s="3"/>
     </row>
     <row r="49" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="B49" s="3"/>
     </row>
     <row r="50" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="B50" s="3"/>
+      <c r="C50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>21</v>
+      <c r="B51" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="E51" s="10">
+        <v>0.1</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C52" s="10">
         <v>0.1</v>
@@ -2845,7 +2844,7 @@
     </row>
     <row r="53" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="C53" s="10">
         <v>0.1</v>
@@ -2859,7 +2858,7 @@
     </row>
     <row r="54" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C54" s="10">
         <v>0.1</v>
@@ -2873,7 +2872,7 @@
     </row>
     <row r="55" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C55" s="10">
         <v>0.1</v>
@@ -2887,7 +2886,7 @@
     </row>
     <row r="56" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C56" s="10">
         <v>0.1</v>
@@ -2901,7 +2900,7 @@
     </row>
     <row r="57" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C57" s="10">
         <v>0.1</v>
@@ -2928,18 +2927,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C59" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D59" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E59" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="B59" s="3"/>
     </row>
     <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
@@ -2948,24 +2936,35 @@
       <c r="B61" s="3"/>
     </row>
     <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="B62" s="3"/>
     </row>
     <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-      <c r="C64" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>21</v>
+      <c r="C64" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="D64" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E64" s="15">
+        <v>0.2</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2973,13 +2972,13 @@
         <v>92</v>
       </c>
       <c r="C65" s="15">
-        <v>0.05</v>
+        <v>0.42</v>
       </c>
       <c r="D65" s="15">
-        <v>2.5000000000000001E-2</v>
+        <v>0.33</v>
       </c>
       <c r="E65" s="15">
-        <v>0.2</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2987,13 +2986,13 @@
         <v>93</v>
       </c>
       <c r="C66" s="15">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="D66" s="15">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="E66" s="15">
-        <v>0.53</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3001,13 +3000,13 @@
         <v>94</v>
       </c>
       <c r="C67" s="15">
-        <v>1</v>
+        <v>2.65</v>
       </c>
       <c r="D67" s="15">
-        <v>0.32</v>
+        <v>1.35</v>
       </c>
       <c r="E67" s="15">
-        <v>1</v>
+        <v>5.19</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3015,13 +3014,13 @@
         <v>95</v>
       </c>
       <c r="C68" s="15">
-        <v>2.65</v>
+        <v>1</v>
       </c>
       <c r="D68" s="15">
+        <v>1</v>
+      </c>
+      <c r="E68" s="15">
         <v>1.35</v>
-      </c>
-      <c r="E68" s="15">
-        <v>5.19</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3029,13 +3028,13 @@
         <v>96</v>
       </c>
       <c r="C69" s="15">
-        <v>1</v>
+        <v>0.46</v>
       </c>
       <c r="D69" s="15">
-        <v>1</v>
+        <v>0.32</v>
       </c>
       <c r="E69" s="15">
-        <v>1.35</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3043,56 +3042,45 @@
         <v>97</v>
       </c>
       <c r="C70" s="15">
-        <v>0.46</v>
+        <v>0.1</v>
       </c>
       <c r="D70" s="15">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E70" s="15">
-        <v>0.67</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>98</v>
+        <v>20</v>
       </c>
       <c r="C71" s="15">
+        <v>0.3</v>
+      </c>
+      <c r="D71" s="15">
         <v>0.1</v>
       </c>
-      <c r="D71" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
       <c r="E71" s="15">
-        <v>0.18</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="C72" s="15">
-        <v>0.3</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="D72" s="15">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E72" s="15">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C73" s="15">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D73" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="E73" s="15">
-        <v>0.35</v>
-      </c>
+      <c r="B73" s="3"/>
     </row>
     <row r="74" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
@@ -3101,24 +3089,35 @@
       <c r="B75" s="3"/>
     </row>
     <row r="76" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="B76" s="3"/>
     </row>
     <row r="77" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="B77" s="3"/>
+      <c r="C77" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-      <c r="C78" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>21</v>
+      <c r="C78" s="9">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D78" s="9">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E78" s="9">
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3126,13 +3125,13 @@
         <v>101</v>
       </c>
       <c r="C79" s="9">
-        <v>0.14599999999999999</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D79" s="9">
-        <v>9.6000000000000002E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E79" s="9">
-        <v>0.20499999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3140,13 +3139,13 @@
         <v>102</v>
       </c>
       <c r="C80" s="9">
-        <v>8.0000000000000002E-3</v>
+        <v>0.02</v>
       </c>
       <c r="D80" s="9">
-        <v>5.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="E80" s="9">
-        <v>1.0999999999999999E-2</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="81" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3154,13 +3153,13 @@
         <v>103</v>
       </c>
       <c r="C81" s="9">
-        <v>0.02</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D81" s="9">
-        <v>1.2999999999999999E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E81" s="9">
-        <v>2.9000000000000001E-2</v>
+        <v>9.4E-2</v>
       </c>
     </row>
     <row r="82" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3168,13 +3167,13 @@
         <v>104</v>
       </c>
       <c r="C82" s="9">
-        <v>7.0000000000000007E-2</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="D82" s="9">
-        <v>4.8000000000000001E-2</v>
+        <v>0.114</v>
       </c>
       <c r="E82" s="9">
-        <v>9.4E-2</v>
+        <v>0.47399999999999998</v>
       </c>
     </row>
     <row r="83" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,13 +3181,13 @@
         <v>105</v>
       </c>
       <c r="C83" s="9">
-        <v>0.26500000000000001</v>
+        <v>0.54700000000000004</v>
       </c>
       <c r="D83" s="9">
-        <v>0.114</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="E83" s="9">
-        <v>0.47399999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
     </row>
     <row r="84" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3196,26 +3195,12 @@
         <v>106</v>
       </c>
       <c r="C84" s="9">
-        <v>0.54700000000000004</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="D84" s="9">
-        <v>0.38200000000000001</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E84" s="9">
-        <v>0.71499999999999997</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="9">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D85" s="9">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="E85" s="9">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
@@ -3429,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3830,8 +3815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4389,8 +4374,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4399,7 +4385,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6287,7 +6273,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
done with spreadsheet, rewriting code now
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="11"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -16,9 +16,8 @@
     <sheet name="Testing &amp; treatment" sheetId="7" r:id="rId7"/>
     <sheet name="Sexual behavior" sheetId="8" r:id="rId8"/>
     <sheet name="Injecting behavior" sheetId="9" r:id="rId9"/>
-    <sheet name="Partnerships" sheetId="10" r:id="rId10"/>
-    <sheet name="Transitions" sheetId="11" r:id="rId11"/>
-    <sheet name="Constants" sheetId="12" r:id="rId12"/>
+    <sheet name="Partnerships &amp; transitions" sheetId="10" r:id="rId10"/>
+    <sheet name="Constants" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -52,40 +51,6 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="Q8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">These values have been calculated in separate spreadsheet provided by Clemens
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="M11" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Reproductive health survey 2010
-	-hassan haghparast</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="P17" authorId="0">
       <text>
         <r>
@@ -114,7 +79,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -164,7 +129,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -187,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="103">
   <si>
     <t>O P T I M A</t>
   </si>
@@ -210,21 +175,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Injects</t>
-  </si>
-  <si>
-    <t>Has sex with men</t>
-  </si>
-  <si>
-    <t>Has sex with women</t>
-  </si>
-  <si>
-    <t>Sex worker</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
     <t>Population size</t>
   </si>
   <si>
@@ -357,9 +307,6 @@
     <t>Interactions between commercial partners</t>
   </si>
   <si>
-    <t>Age-related population transitions (average number of years before movement)</t>
-  </si>
-  <si>
     <t>Interactions between people who inject drugs</t>
   </si>
   <si>
@@ -441,12 +388,6 @@
     <t>CD4(&lt;50) to CD4(50-200)</t>
   </si>
   <si>
-    <t>Treatment failure rate (% per year)</t>
-  </si>
-  <si>
-    <t>First-line treatment</t>
-  </si>
-  <si>
     <t>Death rate (% mortality per year)</t>
   </si>
   <si>
@@ -471,12 +412,6 @@
     <t>Diagnosis behavior change</t>
   </si>
   <si>
-    <t>Ulcerative STI cofactor increase</t>
-  </si>
-  <si>
-    <t>Discharging STI cofactor increase</t>
-  </si>
-  <si>
     <t>Opiate substitution therapy</t>
   </si>
   <si>
@@ -514,16 +449,39 @@
   </si>
   <si>
     <t>For further details please visit: http://optimamodel.com/file/indicator-guide</t>
+  </si>
+  <si>
+    <t>Age range</t>
+  </si>
+  <si>
+    <t>15-49</t>
+  </si>
+  <si>
+    <t>Modeled estimate of number of PLHIV</t>
+  </si>
+  <si>
+    <t>STI cofactor increase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="20"/>
@@ -563,8 +521,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -607,6 +586,12 @@
         <bgColor rgb="FF8064A2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF18C1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -639,56 +624,265 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="10" fontId="1" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="104">
+    <cellStyle name="Comma 2" xfId="4"/>
+    <cellStyle name="Comma 3" xfId="2"/>
+    <cellStyle name="Followed Hyperlink 10" xfId="15"/>
+    <cellStyle name="Followed Hyperlink 11" xfId="16"/>
+    <cellStyle name="Followed Hyperlink 12" xfId="17"/>
+    <cellStyle name="Followed Hyperlink 13" xfId="18"/>
+    <cellStyle name="Followed Hyperlink 14" xfId="19"/>
+    <cellStyle name="Followed Hyperlink 15" xfId="20"/>
+    <cellStyle name="Followed Hyperlink 16" xfId="21"/>
+    <cellStyle name="Followed Hyperlink 17" xfId="22"/>
+    <cellStyle name="Followed Hyperlink 18" xfId="23"/>
+    <cellStyle name="Followed Hyperlink 19" xfId="24"/>
+    <cellStyle name="Followed Hyperlink 2" xfId="7"/>
+    <cellStyle name="Followed Hyperlink 20" xfId="25"/>
+    <cellStyle name="Followed Hyperlink 21" xfId="26"/>
+    <cellStyle name="Followed Hyperlink 22" xfId="27"/>
+    <cellStyle name="Followed Hyperlink 23" xfId="28"/>
+    <cellStyle name="Followed Hyperlink 24" xfId="29"/>
+    <cellStyle name="Followed Hyperlink 25" xfId="30"/>
+    <cellStyle name="Followed Hyperlink 26" xfId="31"/>
+    <cellStyle name="Followed Hyperlink 27" xfId="32"/>
+    <cellStyle name="Followed Hyperlink 28" xfId="33"/>
+    <cellStyle name="Followed Hyperlink 29" xfId="34"/>
+    <cellStyle name="Followed Hyperlink 3" xfId="8"/>
+    <cellStyle name="Followed Hyperlink 30" xfId="35"/>
+    <cellStyle name="Followed Hyperlink 31" xfId="36"/>
+    <cellStyle name="Followed Hyperlink 32" xfId="37"/>
+    <cellStyle name="Followed Hyperlink 33" xfId="38"/>
+    <cellStyle name="Followed Hyperlink 34" xfId="39"/>
+    <cellStyle name="Followed Hyperlink 35" xfId="40"/>
+    <cellStyle name="Followed Hyperlink 36" xfId="41"/>
+    <cellStyle name="Followed Hyperlink 37" xfId="42"/>
+    <cellStyle name="Followed Hyperlink 38" xfId="43"/>
+    <cellStyle name="Followed Hyperlink 39" xfId="44"/>
+    <cellStyle name="Followed Hyperlink 4" xfId="9"/>
+    <cellStyle name="Followed Hyperlink 40" xfId="45"/>
+    <cellStyle name="Followed Hyperlink 41" xfId="46"/>
+    <cellStyle name="Followed Hyperlink 42" xfId="47"/>
+    <cellStyle name="Followed Hyperlink 43" xfId="48"/>
+    <cellStyle name="Followed Hyperlink 44" xfId="49"/>
+    <cellStyle name="Followed Hyperlink 45" xfId="50"/>
+    <cellStyle name="Followed Hyperlink 46" xfId="51"/>
+    <cellStyle name="Followed Hyperlink 47" xfId="52"/>
+    <cellStyle name="Followed Hyperlink 48" xfId="53"/>
+    <cellStyle name="Followed Hyperlink 49" xfId="54"/>
+    <cellStyle name="Followed Hyperlink 5" xfId="10"/>
+    <cellStyle name="Followed Hyperlink 50" xfId="55"/>
+    <cellStyle name="Followed Hyperlink 51" xfId="56"/>
+    <cellStyle name="Followed Hyperlink 52" xfId="57"/>
+    <cellStyle name="Followed Hyperlink 53" xfId="58"/>
+    <cellStyle name="Followed Hyperlink 54" xfId="59"/>
+    <cellStyle name="Followed Hyperlink 55" xfId="60"/>
+    <cellStyle name="Followed Hyperlink 56" xfId="61"/>
+    <cellStyle name="Followed Hyperlink 57" xfId="62"/>
+    <cellStyle name="Followed Hyperlink 58" xfId="63"/>
+    <cellStyle name="Followed Hyperlink 59" xfId="64"/>
+    <cellStyle name="Followed Hyperlink 6" xfId="11"/>
+    <cellStyle name="Followed Hyperlink 60" xfId="65"/>
+    <cellStyle name="Followed Hyperlink 61" xfId="66"/>
+    <cellStyle name="Followed Hyperlink 62" xfId="67"/>
+    <cellStyle name="Followed Hyperlink 63" xfId="68"/>
+    <cellStyle name="Followed Hyperlink 64" xfId="69"/>
+    <cellStyle name="Followed Hyperlink 65" xfId="70"/>
+    <cellStyle name="Followed Hyperlink 66" xfId="71"/>
+    <cellStyle name="Followed Hyperlink 67" xfId="72"/>
+    <cellStyle name="Followed Hyperlink 68" xfId="73"/>
+    <cellStyle name="Followed Hyperlink 69" xfId="74"/>
+    <cellStyle name="Followed Hyperlink 7" xfId="12"/>
+    <cellStyle name="Followed Hyperlink 70" xfId="75"/>
+    <cellStyle name="Followed Hyperlink 71" xfId="76"/>
+    <cellStyle name="Followed Hyperlink 72" xfId="77"/>
+    <cellStyle name="Followed Hyperlink 73" xfId="78"/>
+    <cellStyle name="Followed Hyperlink 74" xfId="79"/>
+    <cellStyle name="Followed Hyperlink 75" xfId="80"/>
+    <cellStyle name="Followed Hyperlink 76" xfId="81"/>
+    <cellStyle name="Followed Hyperlink 77" xfId="82"/>
+    <cellStyle name="Followed Hyperlink 78" xfId="83"/>
+    <cellStyle name="Followed Hyperlink 79" xfId="84"/>
+    <cellStyle name="Followed Hyperlink 8" xfId="13"/>
+    <cellStyle name="Followed Hyperlink 80" xfId="85"/>
+    <cellStyle name="Followed Hyperlink 81" xfId="86"/>
+    <cellStyle name="Followed Hyperlink 82" xfId="87"/>
+    <cellStyle name="Followed Hyperlink 83" xfId="88"/>
+    <cellStyle name="Followed Hyperlink 84" xfId="89"/>
+    <cellStyle name="Followed Hyperlink 85" xfId="90"/>
+    <cellStyle name="Followed Hyperlink 86" xfId="91"/>
+    <cellStyle name="Followed Hyperlink 87" xfId="92"/>
+    <cellStyle name="Followed Hyperlink 88" xfId="93"/>
+    <cellStyle name="Followed Hyperlink 89" xfId="94"/>
+    <cellStyle name="Followed Hyperlink 9" xfId="14"/>
+    <cellStyle name="Followed Hyperlink 90" xfId="95"/>
+    <cellStyle name="Followed Hyperlink 91" xfId="96"/>
+    <cellStyle name="Followed Hyperlink 92" xfId="97"/>
+    <cellStyle name="Followed Hyperlink 93" xfId="98"/>
+    <cellStyle name="Followed Hyperlink 94" xfId="99"/>
+    <cellStyle name="Followed Hyperlink 95" xfId="100"/>
+    <cellStyle name="Followed Hyperlink 96" xfId="101"/>
+    <cellStyle name="Followed Hyperlink 97" xfId="102"/>
+    <cellStyle name="Followed Hyperlink 98" xfId="103"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5"/>
+    <cellStyle name="Normal 3" xfId="6"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Percent 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1952,15 +2146,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
+      <c r="A2" s="24"/>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
     </row>
     <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
@@ -1974,8 +2168,8 @@
       <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
-        <v>108</v>
+      <c r="A7" s="21" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1988,9 +2182,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2001,7 +2197,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2023,7 +2219,7 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2031,9 +2227,7 @@
         <f>Populations!$C$4</f>
         <v>Females 15-49</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2050,7 +2244,7 @@
     </row>
     <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2071,7 +2265,9 @@
         <v>Males 15-49</v>
       </c>
       <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
@@ -2095,7 +2291,7 @@
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2140,7 +2336,7 @@
     </row>
     <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2170,6 +2366,47 @@
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
+    </row>
+    <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>Males 15-49</v>
+      </c>
+      <c r="D30" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>Females 15-49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="7" t="str">
+        <f>Populations!$C$3</f>
+        <v>Males 15-49</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="str">
+        <f>Populations!$C$4</f>
+        <v>Females 15-49</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2178,161 +2415,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="6" width="8.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
-      </c>
-      <c r="D2" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
-      </c>
-      <c r="D9" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="str">
-        <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="str">
-        <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="3:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="3:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="3:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="3:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E84"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
@@ -2341,25 +2430,25 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" s="10">
         <v>4.0000000000000002E-4</v>
@@ -2373,7 +2462,7 @@
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C4" s="10">
         <v>8.0000000000000004E-4</v>
@@ -2387,7 +2476,7 @@
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" s="10">
         <v>1.38E-2</v>
@@ -2401,7 +2490,7 @@
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C6" s="10">
         <v>1.1000000000000001E-3</v>
@@ -2415,7 +2504,7 @@
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C7" s="10">
         <v>8.0000000000000002E-3</v>
@@ -2429,7 +2518,7 @@
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C8" s="10">
         <v>0.36699999999999999</v>
@@ -2443,7 +2532,7 @@
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C9" s="10">
         <v>0.20499999999999999</v>
@@ -2466,25 +2555,25 @@
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C15" s="9">
         <v>26.03</v>
@@ -2498,7 +2587,7 @@
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -2512,7 +2601,7 @@
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
@@ -2526,7 +2615,7 @@
     </row>
     <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -2540,7 +2629,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C19" s="9">
         <v>3.49</v>
@@ -2554,7 +2643,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" s="9">
         <v>7.17</v>
@@ -2577,25 +2666,25 @@
     </row>
     <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C26" s="15">
         <v>4.1399999999999997</v>
@@ -2609,7 +2698,7 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C27" s="15">
         <v>1.05</v>
@@ -2623,7 +2712,7 @@
     </row>
     <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C28" s="15">
         <v>0.33</v>
@@ -2637,7 +2726,7 @@
     </row>
     <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C29" s="15">
         <v>0.27</v>
@@ -2651,7 +2740,7 @@
     </row>
     <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C30" s="15">
         <v>0.67</v>
@@ -2674,25 +2763,25 @@
     </row>
     <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C36" s="15">
         <v>0.45</v>
@@ -2706,7 +2795,7 @@
     </row>
     <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C37" s="15">
         <v>0.7</v>
@@ -2720,7 +2809,7 @@
     </row>
     <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C38" s="15">
         <v>0.47</v>
@@ -2734,7 +2823,7 @@
     </row>
     <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C39" s="15">
         <v>1.52</v>
@@ -2757,450 +2846,395 @@
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="D45" s="15">
-        <v>0.08</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0.12</v>
+        <v>62</v>
+      </c>
+      <c r="C45" s="25">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D45" s="25">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E45" s="25">
+        <v>4.4000000000000003E-3</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="3"/>
+      <c r="B46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="25">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D46" s="25">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E46" s="25">
+        <v>4.4000000000000003E-3</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="3"/>
+      <c r="B47" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="25">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D47" s="25">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="E47" s="25">
+        <v>7.1000000000000004E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
+      <c r="B48" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="25">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="D48" s="25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E48" s="25">
+        <v>1.01E-2</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="3"/>
+      <c r="B49" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="25">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="D49" s="25">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E49" s="25">
+        <v>7.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="50" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-      <c r="C50" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>21</v>
+      <c r="B50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="25">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="D50" s="25">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E50" s="25">
+        <v>0.432</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D51" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E51" s="10">
-        <v>0.1</v>
+        <v>80</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0.23</v>
+      </c>
+      <c r="D51" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="E51" s="25">
+        <v>0.3</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D52" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E52" s="10">
-        <v>0.1</v>
+        <v>81</v>
+      </c>
+      <c r="C52" s="25">
+        <v>2.17</v>
+      </c>
+      <c r="D52" s="25">
+        <v>1.27</v>
+      </c>
+      <c r="E52" s="25">
+        <v>3.71</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D53" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E53" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="B53" s="3"/>
     </row>
     <row r="54" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D54" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E54" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="B54" s="3"/>
     </row>
     <row r="55" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D55" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E55" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="B55" s="3"/>
     </row>
     <row r="56" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D56" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E56" s="10">
-        <v>0.1</v>
-      </c>
+      <c r="A56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="D57" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E57" s="10">
-        <v>0.1</v>
+      <c r="B57" s="3"/>
+      <c r="C57" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="10">
+        <v>83</v>
+      </c>
+      <c r="C58" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="D58" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C59" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="D59" s="15">
+        <v>0.33</v>
+      </c>
+      <c r="E59" s="15">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C60" s="15">
+        <v>1</v>
+      </c>
+      <c r="D60" s="15">
+        <v>0.32</v>
+      </c>
+      <c r="E60" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="15">
+        <v>2.65</v>
+      </c>
+      <c r="D61" s="15">
+        <v>1.35</v>
+      </c>
+      <c r="E61" s="15">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="15">
+        <v>0.46</v>
+      </c>
+      <c r="D62" s="15">
+        <v>0.32</v>
+      </c>
+      <c r="E62" s="15">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="15">
         <v>0.1</v>
       </c>
-      <c r="D58" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="E58" s="10">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-      <c r="C63" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>21</v>
+      <c r="D63" s="15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.18</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="C64" s="15">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="D64" s="15">
-        <v>2.5000000000000001E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E64" s="15">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C65" s="15">
-        <v>0.42</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="D65" s="15">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E65" s="15">
-        <v>0.53</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C66" s="15">
-        <v>1</v>
-      </c>
-      <c r="D66" s="15">
-        <v>0.32</v>
-      </c>
-      <c r="E66" s="15">
-        <v>1</v>
-      </c>
+      <c r="B66" s="3"/>
     </row>
     <row r="67" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C67" s="15">
-        <v>2.65</v>
-      </c>
-      <c r="D67" s="15">
-        <v>1.35</v>
-      </c>
-      <c r="E67" s="15">
-        <v>5.19</v>
-      </c>
+      <c r="B67" s="3"/>
     </row>
     <row r="68" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C68" s="15">
-        <v>1</v>
-      </c>
-      <c r="D68" s="15">
-        <v>1</v>
-      </c>
-      <c r="E68" s="15">
-        <v>1.35</v>
-      </c>
+      <c r="B68" s="3"/>
     </row>
     <row r="69" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="15">
-        <v>0.46</v>
-      </c>
-      <c r="D69" s="15">
-        <v>0.32</v>
-      </c>
-      <c r="E69" s="15">
-        <v>0.67</v>
-      </c>
+      <c r="A69" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="D70" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E70" s="15">
-        <v>0.18</v>
+      <c r="B70" s="3"/>
+      <c r="C70" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="D71" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E71" s="15">
-        <v>0.5</v>
+        <v>90</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="D71" s="9">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E71" s="9">
+        <v>0.20499999999999999</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C72" s="15">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D72" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="E72" s="15">
-        <v>0.35</v>
+        <v>91</v>
+      </c>
+      <c r="C72" s="9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D72" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E72" s="9">
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
+      <c r="B73" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="D73" s="9">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E73" s="9">
+        <v>2.9000000000000001E-2</v>
+      </c>
     </row>
     <row r="74" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
+      <c r="B74" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" s="9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D74" s="9">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E74" s="9">
+        <v>9.4E-2</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
+      <c r="B75" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D75" s="9">
+        <v>0.114</v>
+      </c>
+      <c r="E75" s="9">
+        <v>0.47399999999999998</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B76" s="3"/>
+      <c r="B76" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C76" s="9">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="D76" s="9">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E76" s="9">
+        <v>0.71499999999999997</v>
+      </c>
     </row>
     <row r="77" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-      <c r="C77" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C78" s="9">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="D78" s="9">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="E78" s="9">
-        <v>0.20499999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C79" s="9">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D79" s="9">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="E79" s="9">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C80" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="D80" s="9">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="E80" s="9">
-        <v>2.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C81" s="9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D81" s="9">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="E81" s="9">
-        <v>9.4E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C82" s="9">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="D82" s="9">
-        <v>0.114</v>
-      </c>
-      <c r="E82" s="9">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C83" s="9">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="D83" s="9">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="E83" s="9">
-        <v>0.71499999999999997</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C84" s="9">
+      <c r="B77" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="9">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D77" s="9">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E84" s="9">
+      <c r="E77" s="9">
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
@@ -3211,10 +3245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3224,23 +3258,17 @@
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
     <col min="5" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3254,156 +3282,93 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3415,7 +3380,7 @@
   <dimension ref="A1:AJ10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3425,7 +3390,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3523,7 +3488,7 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3532,11 +3497,9 @@
         <v>Males 15-49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="8">
-        <v>40000</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -3568,7 +3531,7 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ3" s="12"/>
     </row>
@@ -3578,10 +3541,10 @@
         <v>Males 15-49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="8">
-        <v>40000</v>
+        <v>525000</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
@@ -3592,7 +3555,10 @@
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="8">
+        <f>D4*(1.03^10)</f>
+        <v>705556.09915566398</v>
+      </c>
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
@@ -3602,7 +3568,10 @@
       <c r="U4" s="13"/>
       <c r="V4" s="13"/>
       <c r="W4" s="13"/>
-      <c r="X4" s="13"/>
+      <c r="X4" s="13">
+        <f>N4*1.02^10</f>
+        <v>860068.94786402199</v>
+      </c>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
       <c r="AA4" s="12"/>
@@ -3614,7 +3583,7 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="12"/>
       <c r="AI4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ4" s="12"/>
     </row>
@@ -3624,11 +3593,9 @@
         <v>Males 15-49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="8">
-        <v>40000</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -3660,7 +3627,7 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ5" s="12"/>
     </row>
@@ -3671,11 +3638,9 @@
         <v>Females 15-49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="12">
-        <v>40000</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -3707,7 +3672,7 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
       <c r="AI7" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ7" s="12"/>
     </row>
@@ -3717,10 +3682,10 @@
         <v>Females 15-49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8" s="12">
-        <v>40000</v>
+        <v>6260000</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -3731,7 +3696,10 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="N8" s="12">
+        <f>D8*1.03^10</f>
+        <v>8412916.5346942022</v>
+      </c>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
@@ -3741,7 +3709,10 @@
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
+      <c r="X8" s="12">
+        <f>N8*1.02^10</f>
+        <v>10255298.311673861</v>
+      </c>
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
       <c r="AA8" s="12"/>
@@ -3753,7 +3724,7 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ8" s="12"/>
     </row>
@@ -3763,11 +3734,9 @@
         <v>Females 15-49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="12">
-        <v>40000</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -3799,7 +3768,7 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="12"/>
       <c r="AI9" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ9" s="12"/>
     </row>
@@ -3812,11 +3781,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3826,7 +3795,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3924,7 +3893,7 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3933,53 +3902,23 @@
         <v>Males 15-49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="J3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R3" s="10">
-        <v>0.01</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -3997,7 +3936,7 @@
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ3" s="10"/>
     </row>
@@ -4007,53 +3946,29 @@
         <v>Males 15-49</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0.01</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D4" s="10"/>
       <c r="E4" s="10">
         <v>0.01</v>
       </c>
-      <c r="F4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.01</v>
-      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.01</v>
-      </c>
+        <v>0.02</v>
+      </c>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
       <c r="L4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R4" s="10">
-        <v>0.01</v>
-      </c>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -4071,7 +3986,7 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ4" s="14"/>
     </row>
@@ -4081,53 +3996,23 @@
         <v>Males 15-49</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="J5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="L5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q5" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R5" s="10">
-        <v>0.01</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -4145,7 +4030,7 @@
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ5" s="10"/>
     </row>
@@ -4156,53 +4041,23 @@
         <v>Females 15-49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="J7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="L7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q7" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R7" s="10">
-        <v>0.01</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
@@ -4220,7 +4075,7 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ7" s="10"/>
     </row>
@@ -4230,52 +4085,28 @@
         <v>Females 15-49</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0.01</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D8" s="10"/>
       <c r="E8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I8" s="10">
-        <v>0.01</v>
-      </c>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
       <c r="J8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P8" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>0.01</v>
-      </c>
+        <v>0.03</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
       <c r="R8" s="10">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
@@ -4294,7 +4125,7 @@
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ8" s="10"/>
     </row>
@@ -4304,53 +4135,23 @@
         <v>Females 15-49</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="G9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="H9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="I9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="J9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="L9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="N9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="O9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="P9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="R9" s="10">
-        <v>0.01</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
@@ -4368,7 +4169,7 @@
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AJ9" s="10"/>
     </row>
@@ -4376,7 +4177,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4385,7 +4185,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4395,7 +4195,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4493,7 +4293,7 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4502,50 +4302,24 @@
         <v>Males 15-49</v>
       </c>
       <c r="C3" s="10">
-        <v>0</v>
-      </c>
-      <c r="D3" s="10">
-        <v>0</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0</v>
-      </c>
-      <c r="F3" s="10">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0</v>
-      </c>
-      <c r="I3" s="10">
-        <v>0</v>
-      </c>
-      <c r="J3" s="10">
-        <v>0</v>
-      </c>
-      <c r="K3" s="10">
-        <v>0</v>
-      </c>
-      <c r="L3" s="10">
-        <v>0</v>
-      </c>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="10">
-        <v>0</v>
-      </c>
-      <c r="N3" s="10">
-        <v>0</v>
-      </c>
-      <c r="O3" s="10">
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="10">
-        <v>0</v>
-      </c>
+        <v>2E-3</v>
+      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -4563,7 +4337,7 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" s="10"/>
     </row>
@@ -4573,50 +4347,24 @@
         <v>Females 15-49</v>
       </c>
       <c r="C4" s="10">
-        <v>0</v>
-      </c>
-      <c r="D4" s="10">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-      <c r="I4" s="10">
-        <v>0</v>
-      </c>
-      <c r="J4" s="10">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="10">
-        <v>0</v>
-      </c>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
       <c r="M4" s="10">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-      <c r="O4" s="10">
-        <v>0</v>
-      </c>
-      <c r="P4" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="10">
-        <v>0</v>
-      </c>
+        <v>2E-3</v>
+      </c>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -4634,7 +4382,7 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI4" s="10"/>
     </row>
@@ -4643,7 +4391,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4741,7 +4489,7 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4781,7 +4529,7 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI10" s="10">
         <v>0.05</v>
@@ -4802,7 +4550,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="14"/>
+      <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
@@ -4824,7 +4572,7 @@
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI11" s="10">
         <v>0.05</v>
@@ -4835,7 +4583,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4933,7 +4681,7 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4975,7 +4723,7 @@
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI17" s="10"/>
     </row>
@@ -5018,7 +4766,7 @@
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI18" s="10"/>
     </row>
@@ -5031,9 +4779,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI33"/>
+  <dimension ref="A1:AI39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5042,7 +4792,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5140,12 +4890,12 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -5179,7 +4929,7 @@
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
       <c r="AH3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" s="9"/>
     </row>
@@ -5188,7 +4938,7 @@
     <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5286,12 +5036,12 @@
         <v>2030</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -5325,7 +5075,7 @@
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI9" s="9"/>
     </row>
@@ -5334,7 +5084,7 @@
     <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5432,12 +5182,12 @@
         <v>2030</v>
       </c>
       <c r="AI14" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -5471,7 +5221,7 @@
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI15" s="9"/>
     </row>
@@ -5480,7 +5230,7 @@
     <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5578,12 +5328,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -5617,7 +5367,7 @@
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI21" s="9"/>
     </row>
@@ -5626,110 +5376,110 @@
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="5">
+      <c r="C26" s="7">
         <v>2000</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="7">
         <v>2001</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="7">
         <v>2002</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="7">
         <v>2003</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="7">
         <v>2004</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="7">
         <v>2005</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="7">
         <v>2006</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="7">
         <v>2007</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="7">
         <v>2008</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26" s="7">
         <v>2009</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="7">
         <v>2010</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="7">
         <v>2011</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="7">
         <v>2012</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P26" s="7">
         <v>2013</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q26" s="7">
         <v>2014</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="7">
         <v>2015</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="7">
         <v>2016</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="7">
         <v>2017</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="7">
         <v>2018</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="7">
         <v>2019</v>
       </c>
-      <c r="W26" s="5">
+      <c r="W26" s="7">
         <v>2020</v>
       </c>
-      <c r="X26" s="5">
+      <c r="X26" s="7">
         <v>2021</v>
       </c>
-      <c r="Y26" s="5">
+      <c r="Y26" s="7">
         <v>2022</v>
       </c>
-      <c r="Z26" s="5">
+      <c r="Z26" s="7">
         <v>2023</v>
       </c>
-      <c r="AA26" s="5">
+      <c r="AA26" s="7">
         <v>2024</v>
       </c>
-      <c r="AB26" s="5">
+      <c r="AB26" s="7">
         <v>2025</v>
       </c>
-      <c r="AC26" s="5">
+      <c r="AC26" s="7">
         <v>2026</v>
       </c>
-      <c r="AD26" s="5">
+      <c r="AD26" s="7">
         <v>2027</v>
       </c>
-      <c r="AE26" s="5">
+      <c r="AE26" s="7">
         <v>2028</v>
       </c>
-      <c r="AF26" s="5">
+      <c r="AF26" s="7">
         <v>2029</v>
       </c>
-      <c r="AG26" s="5">
+      <c r="AG26" s="7">
         <v>2030</v>
       </c>
-      <c r="AI26" s="5" t="s">
-        <v>14</v>
+      <c r="AI26" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>23</v>
+      <c r="B27" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -5763,7 +5513,7 @@
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI27" s="9"/>
     </row>
@@ -5772,7 +5522,7 @@
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5870,12 +5620,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -5909,9 +5659,155 @@
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI33" s="9"/>
+    </row>
+    <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="5">
+        <v>2000</v>
+      </c>
+      <c r="D38" s="5">
+        <v>2001</v>
+      </c>
+      <c r="E38" s="5">
+        <v>2002</v>
+      </c>
+      <c r="F38" s="5">
+        <v>2003</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2004</v>
+      </c>
+      <c r="H38" s="5">
+        <v>2005</v>
+      </c>
+      <c r="I38" s="5">
+        <v>2006</v>
+      </c>
+      <c r="J38" s="5">
+        <v>2007</v>
+      </c>
+      <c r="K38" s="5">
+        <v>2008</v>
+      </c>
+      <c r="L38" s="5">
+        <v>2009</v>
+      </c>
+      <c r="M38" s="5">
+        <v>2010</v>
+      </c>
+      <c r="N38" s="5">
+        <v>2011</v>
+      </c>
+      <c r="O38" s="5">
+        <v>2012</v>
+      </c>
+      <c r="P38" s="5">
+        <v>2013</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>2014</v>
+      </c>
+      <c r="R38" s="5">
+        <v>2015</v>
+      </c>
+      <c r="S38" s="5">
+        <v>2016</v>
+      </c>
+      <c r="T38" s="5">
+        <v>2017</v>
+      </c>
+      <c r="U38" s="5">
+        <v>2018</v>
+      </c>
+      <c r="V38" s="5">
+        <v>2019</v>
+      </c>
+      <c r="W38" s="5">
+        <v>2020</v>
+      </c>
+      <c r="X38" s="5">
+        <v>2021</v>
+      </c>
+      <c r="Y38" s="5">
+        <v>2022</v>
+      </c>
+      <c r="Z38" s="5">
+        <v>2023</v>
+      </c>
+      <c r="AA38" s="5">
+        <v>2024</v>
+      </c>
+      <c r="AB38" s="5">
+        <v>2025</v>
+      </c>
+      <c r="AC38" s="5">
+        <v>2026</v>
+      </c>
+      <c r="AD38" s="5">
+        <v>2027</v>
+      </c>
+      <c r="AE38" s="5">
+        <v>2028</v>
+      </c>
+      <c r="AF38" s="5">
+        <v>2029</v>
+      </c>
+      <c r="AG38" s="5">
+        <v>2030</v>
+      </c>
+      <c r="AI38" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="9"/>
+      <c r="Y39" s="9"/>
+      <c r="Z39" s="9"/>
+      <c r="AA39" s="9"/>
+      <c r="AB39" s="9"/>
+      <c r="AC39" s="9"/>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI39" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5923,7 +5819,7 @@
   <dimension ref="A1:AI41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5933,7 +5829,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6031,7 +5927,7 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6073,7 +5969,7 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" s="15"/>
     </row>
@@ -6116,7 +6012,7 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
       <c r="AH4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI4" s="15"/>
     </row>
@@ -6125,7 +6021,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6223,12 +6119,12 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -6262,7 +6158,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI10" s="16">
         <v>0.65</v>
@@ -6273,7 +6169,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6371,12 +6267,12 @@
         <v>2030</v>
       </c>
       <c r="AI15" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -6384,18 +6280,26 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="G16" s="6">
+        <v>50</v>
+      </c>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="J16" s="6">
+        <v>600</v>
+      </c>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
+      <c r="O16" s="6">
+        <v>1900</v>
+      </c>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
+      <c r="R16" s="6">
+        <v>3200</v>
+      </c>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -6412,7 +6316,7 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI16" s="6"/>
     </row>
@@ -6421,7 +6325,7 @@
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6519,7 +6423,7 @@
         <v>2030</v>
       </c>
       <c r="AI21" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6527,48 +6431,20 @@
         <f>Populations!$C$3</f>
         <v>Males 15-49</v>
       </c>
-      <c r="C22" s="15">
-        <v>0</v>
-      </c>
-      <c r="D22" s="15">
-        <v>0</v>
-      </c>
-      <c r="E22" s="15">
-        <v>0</v>
-      </c>
-      <c r="F22" s="15">
-        <v>0</v>
-      </c>
-      <c r="G22" s="15">
-        <v>0</v>
-      </c>
-      <c r="H22" s="15">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15">
-        <v>0</v>
-      </c>
-      <c r="K22" s="15">
-        <v>0</v>
-      </c>
-      <c r="L22" s="15">
-        <v>0</v>
-      </c>
-      <c r="M22" s="15">
-        <v>0</v>
-      </c>
-      <c r="N22" s="15">
-        <v>0</v>
-      </c>
-      <c r="O22" s="15">
-        <v>0</v>
-      </c>
-      <c r="P22" s="15">
-        <v>0</v>
-      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
       <c r="Q22" s="15">
         <v>0</v>
       </c>
@@ -6589,7 +6465,7 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="15"/>
       <c r="AH22" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI22" s="15"/>
     </row>
@@ -6598,48 +6474,20 @@
         <f>Populations!$C$4</f>
         <v>Females 15-49</v>
       </c>
-      <c r="C23" s="15">
-        <v>0</v>
-      </c>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15">
-        <v>0</v>
-      </c>
-      <c r="F23" s="15">
-        <v>0</v>
-      </c>
-      <c r="G23" s="15">
-        <v>0</v>
-      </c>
-      <c r="H23" s="15">
-        <v>0</v>
-      </c>
-      <c r="I23" s="15">
-        <v>0</v>
-      </c>
-      <c r="J23" s="15">
-        <v>0</v>
-      </c>
-      <c r="K23" s="15">
-        <v>0</v>
-      </c>
-      <c r="L23" s="15">
-        <v>0</v>
-      </c>
-      <c r="M23" s="15">
-        <v>0</v>
-      </c>
-      <c r="N23" s="15">
-        <v>0</v>
-      </c>
-      <c r="O23" s="15">
-        <v>0</v>
-      </c>
-      <c r="P23" s="15">
-        <v>0</v>
-      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
       <c r="Q23" s="15">
         <v>0</v>
       </c>
@@ -6660,7 +6508,7 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>
       <c r="AH23" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI23" s="15"/>
     </row>
@@ -6669,7 +6517,7 @@
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6767,12 +6615,12 @@
         <v>2030</v>
       </c>
       <c r="AI28" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -6816,7 +6664,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI29" s="6"/>
     </row>
@@ -6825,7 +6673,7 @@
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6923,7 +6771,7 @@
         <v>2030</v>
       </c>
       <c r="AI34" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6989,7 +6837,7 @@
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
       <c r="AH35" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI35" s="9"/>
     </row>
@@ -6998,7 +6846,7 @@
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7096,12 +6944,12 @@
         <v>2030</v>
       </c>
       <c r="AI40" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -7135,7 +6983,7 @@
       <c r="AF41" s="15"/>
       <c r="AG41" s="15"/>
       <c r="AH41" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI41" s="18">
         <f>14/100*87/100</f>
@@ -7153,7 +7001,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AI18" sqref="AI18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7162,7 +7012,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7260,7 +7110,7 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7300,7 +7150,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" s="17">
         <f t="shared" ref="AI3:AI4" si="0">90*60%</f>
@@ -7344,7 +7194,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI4" s="17">
         <f t="shared" si="0"/>
@@ -7356,7 +7206,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7454,7 +7304,7 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7494,7 +7344,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI10" s="17">
         <f>20%*3*20</f>
@@ -7538,7 +7388,7 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI11" s="17">
         <f>10%*3*20</f>
@@ -7550,7 +7400,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7648,7 +7498,7 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7688,10 +7538,10 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI17" s="6">
-        <v>32.585383882974121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7731,7 +7581,7 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI18" s="6">
         <v>0</v>
@@ -7742,7 +7592,7 @@
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7840,7 +7690,7 @@
         <v>2030</v>
       </c>
       <c r="AI23" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7880,7 +7730,7 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI24" s="19">
         <v>0.14000000000000001</v>
@@ -7923,7 +7773,7 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI25" s="19">
         <v>0.14000000000000001</v>
@@ -7934,7 +7784,7 @@
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8032,7 +7882,7 @@
         <v>2030</v>
       </c>
       <c r="AI30" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8072,7 +7922,7 @@
       <c r="AF31" s="15"/>
       <c r="AG31" s="15"/>
       <c r="AH31" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI31" s="15">
         <v>0.28799999999999998</v>
@@ -8115,7 +7965,7 @@
       <c r="AF32" s="15"/>
       <c r="AG32" s="15"/>
       <c r="AH32" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI32" s="15">
         <v>0.28799999999999998</v>
@@ -8126,7 +7976,7 @@
     <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8224,7 +8074,7 @@
         <v>2030</v>
       </c>
       <c r="AI37" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8264,7 +8114,7 @@
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI38" s="20">
         <v>0</v>
@@ -8307,7 +8157,7 @@
       <c r="AF39" s="15"/>
       <c r="AG39" s="15"/>
       <c r="AH39" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI39" s="19">
         <v>0</v>
@@ -8318,7 +8168,7 @@
     <row r="42" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8416,7 +8266,7 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8456,7 +8306,7 @@
       <c r="AF45" s="15"/>
       <c r="AG45" s="15"/>
       <c r="AH45" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI45" s="19">
         <v>0</v>
@@ -8484,7 +8334,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8582,7 +8432,7 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8622,7 +8472,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI3" s="6">
         <v>0</v>
@@ -8665,7 +8515,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI4" s="6">
         <v>0</v>
@@ -8676,7 +8526,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8774,7 +8624,7 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8814,7 +8664,7 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI10" s="15">
         <v>0</v>
@@ -8857,7 +8707,7 @@
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
       <c r="AH11" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI11" s="15">
         <v>0</v>
@@ -8868,7 +8718,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8966,12 +8816,12 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>23</v>
+      <c r="B17" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -9005,7 +8855,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
all working, including error checking
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -3247,7 +3247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -3785,7 +3785,7 @@
   <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4184,8 +4184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added more tests to loadspreadsheet()
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="2"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -2162,8 +2162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2395,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3226,7 +3226,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3357,8 +3357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4161,7 +4161,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
modified cd4transnorm assumption -- not sure whats best
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="9"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -2162,7 +2162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -6978,8 +6978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AI18" sqref="AI18"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7130,8 +7130,7 @@
         <v>19</v>
       </c>
       <c r="AI3" s="17">
-        <f t="shared" ref="AI3:AI4" si="0">90*60%</f>
-        <v>54</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7174,8 +7173,7 @@
         <v>19</v>
       </c>
       <c r="AI4" s="17">
-        <f t="shared" si="0"/>
-        <v>54</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change to spreadsheet layout
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="7"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -378,9 +378,6 @@
     <t>Tuberculosis cofactor</t>
   </si>
   <si>
-    <t>Relative transmissibility</t>
-  </si>
-  <si>
     <t>Condom use</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>STI cofactor increase</t>
+  </si>
+  <si>
+    <t>Change in transmissibility</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -755,6 +755,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="104">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2147,7 +2148,7 @@
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2393,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2896,7 +2897,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>66</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>67</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>0.432</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>80</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>81</v>
       </c>
@@ -2952,22 +2953,22 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="5" t="s">
         <v>25</v>
@@ -2979,134 +2980,158 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="D58" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="G58" s="26"/>
+      <c r="H58" s="26"/>
+      <c r="I58" s="26"/>
+    </row>
+    <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="D59" s="15">
+        <v>0.82000000000000006</v>
+      </c>
+      <c r="E59" s="15">
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+    </row>
+    <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="15">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="D60" s="15">
+        <v>0.65</v>
+      </c>
+      <c r="E60" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+    </row>
+    <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C61" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="D61" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="E61" s="15">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+    </row>
+    <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C58" s="15">
-        <v>0.05</v>
-      </c>
-      <c r="D58" s="15">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="E58" s="15">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+      <c r="C62" s="15">
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="D62" s="15">
+        <v>0.47</v>
+      </c>
+      <c r="E62" s="15">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+    </row>
+    <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" s="15">
+        <v>0.54</v>
+      </c>
+      <c r="D63" s="15">
+        <v>0.32999999999999996</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+    </row>
+    <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C59" s="15">
-        <v>0.42</v>
-      </c>
-      <c r="D59" s="15">
-        <v>0.33</v>
-      </c>
-      <c r="E59" s="15">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" s="15">
-        <v>1</v>
-      </c>
-      <c r="D60" s="15">
-        <v>0.32</v>
-      </c>
-      <c r="E60" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="15">
+      <c r="C64" s="15">
+        <v>0</v>
+      </c>
+      <c r="D64" s="15">
+        <v>0</v>
+      </c>
+      <c r="E64" s="15">
+        <v>0.67999999999999994</v>
+      </c>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+    </row>
+    <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C65" s="15">
         <v>2.65</v>
       </c>
-      <c r="D61" s="15">
+      <c r="D65" s="15">
         <v>1.35</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E65" s="15">
         <v>5.19</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" s="15">
-        <v>0.46</v>
-      </c>
-      <c r="D62" s="15">
-        <v>0.32</v>
-      </c>
-      <c r="E62" s="15">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="D63" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E63" s="15">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C64" s="15">
-        <v>0.3</v>
-      </c>
-      <c r="D64" s="15">
-        <v>0.1</v>
-      </c>
-      <c r="E64" s="15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+    </row>
+    <row r="66" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C65" s="15">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="D65" s="15">
-        <v>0.2</v>
-      </c>
-      <c r="E65" s="15">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="5" t="s">
         <v>25</v>
@@ -3118,9 +3143,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" s="9">
         <v>0.14599999999999999</v>
@@ -3132,9 +3157,9 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" s="9">
         <v>8.0000000000000002E-3</v>
@@ -3146,9 +3171,9 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" s="9">
         <v>0.02</v>
@@ -3160,9 +3185,9 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" s="9">
         <v>7.0000000000000007E-2</v>
@@ -3174,9 +3199,9 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="9">
         <v>0.26500000000000001</v>
@@ -3188,9 +3213,9 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" s="9">
         <v>0.54700000000000004</v>
@@ -3202,9 +3227,9 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="9">
         <v>5.2999999999999999E-2</v>
@@ -3260,7 +3285,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3280,7 +3305,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3300,7 +3325,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5353,7 +5378,7 @@
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6146,7 +6171,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6978,7 +7003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
untitled for now, but maybe useful for testing later
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="10"/>
+    <workbookView xWindow="210" yWindow="390" windowWidth="28440" windowHeight="12450" tabRatio="861" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="16" r:id="rId1"/>
@@ -2396,8 +2396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7003,8 +7003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" topLeftCell="N4" workbookViewId="0">
+      <selection activeCell="AI27" sqref="AI27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7925,7 +7925,7 @@
         <v>19</v>
       </c>
       <c r="AI31" s="15">
-        <v>0.28799999999999998</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7968,7 +7968,7 @@
         <v>19</v>
       </c>
       <c r="AI32" s="15">
-        <v>0.28799999999999998</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
program tests dont work, but closer
</commit_message>
<xml_diff>
--- a/optima/test.xlsx
+++ b/optima/test.xlsx
@@ -156,9 +156,6 @@
     <t>Population size</t>
   </si>
   <si>
-    <t>Males 15-49</t>
-  </si>
-  <si>
     <t>Assumption</t>
   </si>
   <si>
@@ -171,9 +168,6 @@
     <t>FALSE</t>
   </si>
   <si>
-    <t>Females 15-49</t>
-  </si>
-  <si>
     <t>Other females (15-49)</t>
   </si>
   <si>
@@ -439,6 +433,12 @@
   </si>
   <si>
     <t>Age to</t>
+  </si>
+  <si>
+    <t>M 15-49</t>
+  </si>
+  <si>
+    <t>F 15-49</t>
   </si>
 </sst>
 </file>
@@ -2148,7 +2148,7 @@
     </row>
     <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2176,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -2184,17 +2184,17 @@
     <row r="2" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="D2" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6">
@@ -2204,7 +2204,7 @@
     <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -2223,7 +2223,7 @@
     </row>
     <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2231,17 +2231,17 @@
     <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="D9" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6">
@@ -2251,7 +2251,7 @@
     <row r="11" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="15" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2278,17 +2278,17 @@
     <row r="16" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="D16" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2296,7 +2296,7 @@
     <row r="18" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="22" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -2323,17 +2323,17 @@
     <row r="23" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="D23" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -2341,14 +2341,14 @@
     <row r="25" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
     <row r="29" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2356,17 +2356,17 @@
     <row r="30" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="D30" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C31" s="6">
         <v>0</v>
@@ -2378,7 +2378,7 @@
     <row r="32" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C32" s="6">
         <v>0</v>
@@ -2409,25 +2409,25 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="C2" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C3" s="10">
         <v>4.0000000000000002E-4</v>
@@ -2441,7 +2441,7 @@
     </row>
     <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="10">
         <v>8.0000000000000004E-4</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C5" s="10">
         <v>1.38E-2</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C6" s="10">
         <v>1.1000000000000001E-3</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="10">
         <v>8.0000000000000002E-3</v>
@@ -2497,7 +2497,7 @@
     </row>
     <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="10">
         <v>0.36699999999999999</v>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" s="10">
         <v>0.20499999999999999</v>
@@ -2534,25 +2534,25 @@
     </row>
     <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="9">
         <v>26.03</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="9">
         <v>1</v>
@@ -2580,7 +2580,7 @@
     </row>
     <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -2608,7 +2608,7 @@
     </row>
     <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="9">
         <v>3.49</v>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="9">
         <v>7.17</v>
@@ -2645,25 +2645,25 @@
     </row>
     <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C26" s="15">
         <v>4.1399999999999997</v>
@@ -2677,7 +2677,7 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C27" s="15">
         <v>1.05</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="15">
         <v>0.33</v>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="15">
         <v>0.27</v>
@@ -2719,7 +2719,7 @@
     </row>
     <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C30" s="15">
         <v>0.67</v>
@@ -2742,25 +2742,25 @@
     </row>
     <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="15">
         <v>0.45</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C37" s="15">
         <v>0.7</v>
@@ -2788,7 +2788,7 @@
     </row>
     <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="15">
         <v>0.47</v>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="15">
         <v>1.52</v>
@@ -2825,25 +2825,25 @@
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C45" s="23">
         <v>3.5999999999999999E-3</v>
@@ -2857,7 +2857,7 @@
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C46" s="23">
         <v>3.5999999999999999E-3</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C47" s="23">
         <v>5.7999999999999996E-3</v>
@@ -2885,7 +2885,7 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C48" s="23">
         <v>8.8000000000000005E-3</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="49" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49" s="23">
         <v>5.8999999999999997E-2</v>
@@ -2913,7 +2913,7 @@
     </row>
     <row r="50" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C50" s="23">
         <v>0.32300000000000001</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="51" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" s="23">
         <v>0.23</v>
@@ -2941,7 +2941,7 @@
     </row>
     <row r="52" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C52" s="23">
         <v>2.17</v>
@@ -2964,25 +2964,25 @@
     </row>
     <row r="56" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C58" s="15">
         <v>0.7</v>
@@ -2999,7 +2999,7 @@
     </row>
     <row r="59" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C59" s="15">
         <v>0.9</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="60" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C60" s="15">
         <v>0.72499999999999998</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="61" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C61" s="15">
         <v>0.95</v>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="62" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C62" s="15">
         <v>0.58000000000000007</v>
@@ -3067,7 +3067,7 @@
     </row>
     <row r="63" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C63" s="15">
         <v>0.54</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="64" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C64" s="15">
         <v>0</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="65" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C65" s="15">
         <v>2.65</v>
@@ -3127,25 +3127,25 @@
     </row>
     <row r="69" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B69" s="3"/>
     </row>
     <row r="70" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C71" s="9">
         <v>0.14599999999999999</v>
@@ -3159,7 +3159,7 @@
     </row>
     <row r="72" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C72" s="9">
         <v>8.0000000000000002E-3</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="73" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C73" s="9">
         <v>0.02</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="74" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C74" s="9">
         <v>7.0000000000000007E-2</v>
@@ -3201,7 +3201,7 @@
     </row>
     <row r="75" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C75" s="9">
         <v>0.26500000000000001</v>
@@ -3215,7 +3215,7 @@
     </row>
     <row r="76" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C76" s="9">
         <v>0.54700000000000004</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C77" s="9">
         <v>5.2999999999999999E-2</v>
@@ -3251,7 +3251,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3285,10 +3285,10 @@
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3296,16 +3296,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>12</v>
       </c>
       <c r="G3" s="6">
         <v>15</v>
@@ -3319,16 +3319,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="6">
         <v>15</v>
@@ -3500,16 +3500,16 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -3543,17 +3543,17 @@
       <c r="AG3" s="12"/>
       <c r="AH3" s="12"/>
       <c r="AI3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ3" s="12"/>
     </row>
     <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="8">
         <v>525000</v>
@@ -3595,17 +3595,17 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="12"/>
       <c r="AI4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ4" s="12"/>
     </row>
     <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
@@ -3639,7 +3639,7 @@
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ5" s="12"/>
     </row>
@@ -3647,10 +3647,10 @@
     <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -3684,17 +3684,17 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
       <c r="AI7" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ7" s="12"/>
     </row>
     <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="12">
         <v>626000</v>
@@ -3736,17 +3736,17 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="12"/>
       <c r="AI8" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ8" s="12"/>
     </row>
     <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -3780,7 +3780,7 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="12"/>
       <c r="AI9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ9" s="12"/>
     </row>
@@ -3806,7 +3806,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3904,16 +3904,16 @@
         <v>2030</v>
       </c>
       <c r="AJ2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -3947,17 +3947,17 @@
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ3" s="10"/>
     </row>
     <row r="4" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10">
@@ -3997,17 +3997,17 @@
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
       <c r="AI4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ4" s="14"/>
     </row>
     <row r="5" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -4041,7 +4041,7 @@
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ5" s="10"/>
     </row>
@@ -4049,10 +4049,10 @@
     <row r="7" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -4086,17 +4086,17 @@
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ7" s="10"/>
     </row>
     <row r="8" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
@@ -4136,17 +4136,17 @@
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
       <c r="AI8" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ8" s="10"/>
     </row>
     <row r="9" spans="1:36" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -4180,7 +4180,7 @@
       <c r="AG9" s="10"/>
       <c r="AH9" s="10"/>
       <c r="AI9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AJ9" s="10"/>
     </row>
@@ -4206,7 +4206,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4304,13 +4304,13 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="10">
         <v>3.0000000000000001E-3</v>
@@ -4348,14 +4348,14 @@
       <c r="AF3" s="10"/>
       <c r="AG3" s="10"/>
       <c r="AH3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI3" s="10"/>
     </row>
     <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C4" s="10">
         <v>3.0000000000000001E-3</v>
@@ -4393,7 +4393,7 @@
       <c r="AF4" s="10"/>
       <c r="AG4" s="10"/>
       <c r="AH4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI4" s="10"/>
     </row>
@@ -4402,7 +4402,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4500,13 +4500,13 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -4540,7 +4540,7 @@
       <c r="AF10" s="10"/>
       <c r="AG10" s="10"/>
       <c r="AH10" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI10" s="10">
         <v>0.05</v>
@@ -4549,7 +4549,7 @@
     <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -4583,7 +4583,7 @@
       <c r="AF11" s="10"/>
       <c r="AG11" s="10"/>
       <c r="AH11" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI11" s="10">
         <v>0.05</v>
@@ -4594,7 +4594,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4692,13 +4692,13 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -4734,14 +4734,14 @@
       <c r="AF17" s="10"/>
       <c r="AG17" s="10"/>
       <c r="AH17" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI17" s="10"/>
     </row>
     <row r="18" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -4777,7 +4777,7 @@
       <c r="AF18" s="10"/>
       <c r="AG18" s="10"/>
       <c r="AH18" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI18" s="10"/>
     </row>
@@ -4803,7 +4803,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4901,12 +4901,12 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -4940,7 +4940,7 @@
       <c r="AF3" s="9"/>
       <c r="AG3" s="9"/>
       <c r="AH3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI3" s="9"/>
     </row>
@@ -4949,7 +4949,7 @@
     <row r="6" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5047,12 +5047,12 @@
         <v>2030</v>
       </c>
       <c r="AI8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -5086,7 +5086,7 @@
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
       <c r="AH9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI9" s="9"/>
     </row>
@@ -5095,7 +5095,7 @@
     <row r="12" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5193,12 +5193,12 @@
         <v>2030</v>
       </c>
       <c r="AI14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -5232,7 +5232,7 @@
       <c r="AF15" s="9"/>
       <c r="AG15" s="9"/>
       <c r="AH15" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI15" s="9"/>
     </row>
@@ -5241,7 +5241,7 @@
     <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5339,12 +5339,12 @@
         <v>2030</v>
       </c>
       <c r="AI20" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -5378,7 +5378,7 @@
       <c r="AF21" s="9"/>
       <c r="AG21" s="9"/>
       <c r="AH21" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI21" s="9"/>
     </row>
@@ -5387,7 +5387,7 @@
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5485,12 +5485,12 @@
         <v>2030</v>
       </c>
       <c r="AI26" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -5524,7 +5524,7 @@
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI27" s="9"/>
     </row>
@@ -5533,7 +5533,7 @@
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5631,12 +5631,12 @@
         <v>2030</v>
       </c>
       <c r="AI32" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
@@ -5670,7 +5670,7 @@
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI33" s="9"/>
     </row>
@@ -5679,7 +5679,7 @@
     <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5777,12 +5777,12 @@
         <v>2030</v>
       </c>
       <c r="AI38" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -5816,7 +5816,7 @@
       <c r="AF39" s="9"/>
       <c r="AG39" s="9"/>
       <c r="AH39" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI39" s="9"/>
     </row>
@@ -5840,7 +5840,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5938,13 +5938,13 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -5980,14 +5980,14 @@
       <c r="AF3" s="15"/>
       <c r="AG3" s="15"/>
       <c r="AH3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI3" s="15"/>
     </row>
     <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
@@ -6023,7 +6023,7 @@
       <c r="AF4" s="15"/>
       <c r="AG4" s="15"/>
       <c r="AH4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI4" s="15"/>
     </row>
@@ -6032,7 +6032,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6130,12 +6130,12 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -6169,7 +6169,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI10" s="16">
         <v>0.65</v>
@@ -6180,7 +6180,7 @@
     <row r="13" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6278,12 +6278,12 @@
         <v>2030</v>
       </c>
       <c r="AI15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
@@ -6327,7 +6327,7 @@
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
       <c r="AH16" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI16" s="6"/>
     </row>
@@ -6336,7 +6336,7 @@
     <row r="19" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6434,13 +6434,13 @@
         <v>2030</v>
       </c>
       <c r="AI21" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -6476,14 +6476,14 @@
       <c r="AF22" s="15"/>
       <c r="AG22" s="15"/>
       <c r="AH22" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI22" s="15"/>
     </row>
     <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -6519,7 +6519,7 @@
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>
       <c r="AH23" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI23" s="15"/>
     </row>
@@ -6528,7 +6528,7 @@
     <row r="26" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6626,12 +6626,12 @@
         <v>2030</v>
       </c>
       <c r="AI28" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
@@ -6675,7 +6675,7 @@
       <c r="AF29" s="6"/>
       <c r="AG29" s="6"/>
       <c r="AH29" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI29" s="6"/>
     </row>
@@ -6684,7 +6684,7 @@
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6782,13 +6782,13 @@
         <v>2030</v>
       </c>
       <c r="AI34" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C35" s="9">
         <v>4.5925296336727484E-2</v>
@@ -6848,7 +6848,7 @@
       <c r="AF35" s="9"/>
       <c r="AG35" s="9"/>
       <c r="AH35" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI35" s="9"/>
     </row>
@@ -6857,7 +6857,7 @@
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6955,12 +6955,12 @@
         <v>2030</v>
       </c>
       <c r="AI40" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C41" s="15"/>
       <c r="D41" s="15"/>
@@ -6994,7 +6994,7 @@
       <c r="AF41" s="15"/>
       <c r="AG41" s="15"/>
       <c r="AH41" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI41" s="18">
         <f>14/100*87/100</f>
@@ -7021,7 +7021,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7119,13 +7119,13 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -7159,7 +7159,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI3" s="17">
         <v>100</v>
@@ -7168,7 +7168,7 @@
     <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -7202,7 +7202,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI4" s="17">
         <v>100</v>
@@ -7213,7 +7213,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7311,13 +7311,13 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -7351,7 +7351,7 @@
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI10" s="17">
         <f>20%*3*20</f>
@@ -7361,7 +7361,7 @@
     <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -7395,7 +7395,7 @@
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI11" s="17">
         <f>10%*3*20</f>
@@ -7407,7 +7407,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7505,13 +7505,13 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -7545,7 +7545,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>
@@ -7554,7 +7554,7 @@
     <row r="18" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -7588,7 +7588,7 @@
       <c r="AF18" s="6"/>
       <c r="AG18" s="6"/>
       <c r="AH18" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI18" s="6">
         <v>0</v>
@@ -7599,7 +7599,7 @@
     <row r="21" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7697,13 +7697,13 @@
         <v>2030</v>
       </c>
       <c r="AI23" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
@@ -7737,7 +7737,7 @@
       <c r="AF24" s="15"/>
       <c r="AG24" s="15"/>
       <c r="AH24" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI24" s="19">
         <v>0.14000000000000001</v>
@@ -7746,7 +7746,7 @@
     <row r="25" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
@@ -7780,7 +7780,7 @@
       <c r="AF25" s="15"/>
       <c r="AG25" s="15"/>
       <c r="AH25" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI25" s="19">
         <v>0.14000000000000001</v>
@@ -7791,7 +7791,7 @@
     <row r="28" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7889,13 +7889,13 @@
         <v>2030</v>
       </c>
       <c r="AI30" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -7929,7 +7929,7 @@
       <c r="AF31" s="15"/>
       <c r="AG31" s="15"/>
       <c r="AH31" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI31" s="15">
         <v>0.3</v>
@@ -7938,7 +7938,7 @@
     <row r="32" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -7972,7 +7972,7 @@
       <c r="AF32" s="15"/>
       <c r="AG32" s="15"/>
       <c r="AH32" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI32" s="15">
         <v>0.4</v>
@@ -7983,7 +7983,7 @@
     <row r="35" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8081,13 +8081,13 @@
         <v>2030</v>
       </c>
       <c r="AI37" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="15"/>
@@ -8121,7 +8121,7 @@
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI38" s="20">
         <v>0</v>
@@ -8130,7 +8130,7 @@
     <row r="39" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
@@ -8164,7 +8164,7 @@
       <c r="AF39" s="15"/>
       <c r="AG39" s="15"/>
       <c r="AH39" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI39" s="19">
         <v>0</v>
@@ -8175,7 +8175,7 @@
     <row r="42" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8273,13 +8273,13 @@
         <v>2030</v>
       </c>
       <c r="AI44" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -8313,7 +8313,7 @@
       <c r="AF45" s="15"/>
       <c r="AG45" s="15"/>
       <c r="AH45" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI45" s="19">
         <v>0</v>
@@ -8341,7 +8341,7 @@
   <sheetData>
     <row r="1" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8439,13 +8439,13 @@
         <v>2030</v>
       </c>
       <c r="AI2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -8479,7 +8479,7 @@
       <c r="AF3" s="6"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI3" s="6">
         <v>0</v>
@@ -8488,7 +8488,7 @@
     <row r="4" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -8522,7 +8522,7 @@
       <c r="AF4" s="6"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI4" s="6">
         <v>0</v>
@@ -8533,7 +8533,7 @@
     <row r="7" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8631,13 +8631,13 @@
         <v>2030</v>
       </c>
       <c r="AI9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="str">
         <f>Populations!$C$3</f>
-        <v>Males 15-49</v>
+        <v>M 15-49</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -8671,7 +8671,7 @@
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI10" s="15">
         <v>0</v>
@@ -8680,7 +8680,7 @@
     <row r="11" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="str">
         <f>Populations!$C$4</f>
-        <v>Females 15-49</v>
+        <v>F 15-49</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -8714,7 +8714,7 @@
       <c r="AF11" s="15"/>
       <c r="AG11" s="15"/>
       <c r="AH11" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI11" s="15">
         <v>0</v>
@@ -8725,7 +8725,7 @@
     <row r="14" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8823,12 +8823,12 @@
         <v>2030</v>
       </c>
       <c r="AI16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -8862,7 +8862,7 @@
       <c r="AF17" s="6"/>
       <c r="AG17" s="6"/>
       <c r="AH17" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AI17" s="6">
         <v>0</v>

</xml_diff>